<commit_message>
update budget with new venue information
</commit_message>
<xml_diff>
--- a/Budget/owasp-devseccon-summit-budget.xlsx
+++ b/Budget/owasp-devseccon-summit-budget.xlsx
@@ -16,15 +16,12 @@
     <sheet name="summit 2017 budget" sheetId="1" r:id="rId2"/>
     <sheet name="Assumptions" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
-  <si>
-    <t>Conference attendees</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Estimated profit</t>
   </si>
@@ -41,21 +38,9 @@
     <t>Final</t>
   </si>
   <si>
-    <t>Venue</t>
-  </si>
-  <si>
-    <t>Conference fee</t>
-  </si>
-  <si>
-    <t>Keynotes expenses</t>
-  </si>
-  <si>
     <t>Sponsorship</t>
   </si>
   <si>
-    <t>Volunteers expenses</t>
-  </si>
-  <si>
     <t>Catering</t>
   </si>
   <si>
@@ -68,18 +53,9 @@
     <t>Social activities</t>
   </si>
   <si>
-    <t>Swag</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
-    <t>Graphic designer</t>
-  </si>
-  <si>
-    <t>Flyers</t>
-  </si>
-  <si>
     <t>Badges</t>
   </si>
   <si>
@@ -95,12 +71,6 @@
     <t># volunteers</t>
   </si>
   <si>
-    <t>cost per volunteer</t>
-  </si>
-  <si>
-    <t># owasp seed</t>
-  </si>
-  <si>
     <t>all budget is in USD</t>
   </si>
   <si>
@@ -113,37 +83,70 @@
     <t>Use numbers based on assumptions to create the budget, so we can update the budget by validating or updating our assumptions</t>
   </si>
   <si>
-    <t># attendees</t>
-  </si>
-  <si>
-    <t>fee per attendee</t>
-  </si>
-  <si>
     <t>number of summit days</t>
   </si>
   <si>
-    <t>cost per hotel room per day</t>
-  </si>
-  <si>
-    <t>catering cost per attendee per day</t>
-  </si>
-  <si>
-    <t>venue cost per day</t>
-  </si>
-  <si>
-    <t>travel per attendee</t>
-  </si>
-  <si>
-    <t>Travel</t>
-  </si>
-  <si>
     <t>seed fund owasp</t>
   </si>
   <si>
     <t>owasp chapters / projects</t>
   </si>
   <si>
-    <t>Current assumption is 75 participants paying 2000 USD</t>
+    <t>people covering own ticket</t>
+  </si>
+  <si>
+    <t>all-in cost per day per person</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>summit ticket</t>
+  </si>
+  <si>
+    <t>owasp seed</t>
+  </si>
+  <si>
+    <t># attendees paying themselves</t>
+  </si>
+  <si>
+    <t># of sponsored attendees</t>
+  </si>
+  <si>
+    <t>Venue - cost (all-in)</t>
+  </si>
+  <si>
+    <t>Sponsored travel</t>
+  </si>
+  <si>
+    <t>average travel per attendee</t>
+  </si>
+  <si>
+    <t>sponsor income</t>
+  </si>
+  <si>
+    <t>project/chapter donactions</t>
+  </si>
+  <si>
+    <t>summit attendees</t>
+  </si>
+  <si>
+    <t>included above</t>
+  </si>
+  <si>
+    <t>social event cost per attendee</t>
+  </si>
+  <si>
+    <t>t-shirts</t>
+  </si>
+  <si>
+    <t>cost of t-shirt</t>
+  </si>
+  <si>
+    <t>website cost (layout/hosting)</t>
+  </si>
+  <si>
+    <t>badge cost</t>
   </si>
 </sst>
 </file>
@@ -154,7 +157,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.###############"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -223,13 +226,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Courier New"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
       <name val="Courier New"/>
     </font>
   </fonts>
@@ -474,7 +470,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -518,6 +513,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -812,22 +810,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="68"/>
+    <col min="1" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
-        <v>27</v>
+      <c r="A1" s="67" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="68" t="s">
-        <v>28</v>
+      <c r="A2" s="67" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="68" t="s">
-        <v>29</v>
+      <c r="A3" s="67" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +838,7 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -870,13 +868,13 @@
     <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="69" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" s="70"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="67">
-        <v>42826</v>
+      <c r="F2" s="66">
+        <v>42887</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="12"/>
@@ -896,15 +894,15 @@
     <row r="4" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="22" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C4" s="23">
-        <f>Assumptions!B7</f>
-        <v>75</v>
+        <f>Assumptions!B3+Assumptions!B6+Assumptions!B7</f>
+        <v>125</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="26">
         <v>0</v>
@@ -919,11 +917,11 @@
       <c r="C5" s="23"/>
       <c r="D5" s="28"/>
       <c r="E5" s="29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="30">
         <f>C27-F27</f>
-        <v>-22375</v>
+        <v>148375</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="7"/>
@@ -943,12 +941,12 @@
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="5"/>
       <c r="E7" s="36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="19"/>
@@ -969,12 +967,12 @@
       <c r="A9" s="14"/>
       <c r="B9" s="40"/>
       <c r="C9" s="41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="42"/>
       <c r="F9" s="41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="32"/>
@@ -983,18 +981,18 @@
     <row r="10" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="43" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C10" s="44">
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="45" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F10" s="46">
-        <f>Assumptions!B8*Assumptions!B11</f>
-        <v>75000</v>
+        <f>(Assumptions!B6+Assumptions!B7)*Assumptions!B8*Assumptions!B9</f>
+        <v>178250</v>
       </c>
       <c r="G10" s="47"/>
       <c r="H10" s="32"/>
@@ -1003,18 +1001,18 @@
     <row r="11" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
       <c r="B11" s="43" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C11" s="44">
-        <f>Assumptions!B7*Assumptions!B6</f>
-        <v>150000</v>
+        <f>Assumptions!B6*Assumptions!B8*Assumptions!B9</f>
+        <v>116250</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="48">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="F11" s="46" t="s">
+        <v>36</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="32"/>
@@ -1023,117 +1021,127 @@
     <row r="12" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
       <c r="B12" s="43" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C12" s="44">
-        <v>0</v>
+        <f>Assumptions!B11</f>
+        <v>30000</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="49">
-        <f>((Assumptions!B10*Assumptions!B8)+Assumptions!B9*(Assumptions!B8+1))*Assumptions!B3</f>
-        <v>9750</v>
+        <v>31</v>
+      </c>
+      <c r="F12" s="48">
+        <f>Assumptions!B7*Assumptions!B10</f>
+        <v>28000</v>
       </c>
       <c r="G12" s="47"/>
       <c r="H12" s="32"/>
       <c r="I12" s="33"/>
     </row>
     <row r="13" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="43" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C13" s="44">
-        <v>0</v>
+        <f>Assumptions!B12</f>
+        <v>75000</v>
       </c>
       <c r="D13" s="27"/>
-      <c r="E13" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="46">
-        <f>Assumptions!B10*Assumptions!B7*Assumptions!B8</f>
-        <v>28125</v>
-      </c>
+      <c r="E13" s="45"/>
+      <c r="F13" s="48"/>
       <c r="G13" s="47"/>
       <c r="H13" s="32"/>
       <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="19"/>
       <c r="E14" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="46"/>
+        <v>7</v>
+      </c>
+      <c r="F14" s="46">
+        <v>1000</v>
+      </c>
       <c r="G14" s="47"/>
       <c r="H14" s="32"/>
       <c r="I14" s="33"/>
     </row>
     <row r="15" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="50"/>
       <c r="D15" s="19"/>
       <c r="E15" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="46"/>
+        <v>8</v>
+      </c>
+      <c r="F15" s="46">
+        <v>1000</v>
+      </c>
       <c r="G15" s="47"/>
       <c r="H15" s="32"/>
       <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="53"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="19"/>
       <c r="E16" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="48"/>
+        <v>9</v>
+      </c>
+      <c r="F16" s="48">
+        <f>(Assumptions!B3+Assumptions!B6+Assumptions!B7)*Assumptions!B13</f>
+        <v>6250</v>
+      </c>
       <c r="G16" s="27"/>
       <c r="H16" s="32"/>
       <c r="I16" s="33"/>
     </row>
     <row r="17" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="19"/>
       <c r="E17" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="48"/>
+        <v>38</v>
+      </c>
+      <c r="F17" s="48">
+        <f>(Assumptions!B3+Assumptions!B7+Assumptions!B6)*Assumptions!B14</f>
+        <v>3750</v>
+      </c>
       <c r="G17" s="27"/>
       <c r="H17" s="32"/>
       <c r="I17" s="33"/>
     </row>
     <row r="18" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
       <c r="D18" s="19"/>
       <c r="E18" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="46"/>
+        <v>10</v>
+      </c>
+      <c r="F18" s="46">
+        <f>Assumptions!B15</f>
+        <v>3000</v>
+      </c>
       <c r="G18" s="27"/>
       <c r="H18" s="32"/>
       <c r="I18" s="33"/>
     </row>
     <row r="19" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="53"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="19"/>
       <c r="E19" s="45" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="F19" s="48">
-        <f>(Assumptions!B3+Assumptions!B7)*Assumptions!B12</f>
-        <v>59500</v>
+        <f>C4*Assumptions!B16</f>
+        <v>625</v>
       </c>
       <c r="G19" s="27"/>
       <c r="H19" s="32"/>
@@ -1141,25 +1149,25 @@
     </row>
     <row r="20" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="53"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="19"/>
       <c r="E20" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="46"/>
+        <v>12</v>
+      </c>
+      <c r="F20" s="46">
+        <v>1000</v>
+      </c>
       <c r="G20" s="27"/>
       <c r="H20" s="32"/>
       <c r="I20" s="33"/>
     </row>
     <row r="21" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="53"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="19"/>
-      <c r="E21" s="45" t="s">
-        <v>18</v>
-      </c>
+      <c r="E21" s="45"/>
       <c r="F21" s="46"/>
       <c r="G21" s="27"/>
       <c r="H21" s="32"/>
@@ -1167,12 +1175,10 @@
     </row>
     <row r="22" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="19"/>
-      <c r="E22" s="45" t="s">
-        <v>19</v>
-      </c>
+      <c r="E22" s="45"/>
       <c r="F22" s="48"/>
       <c r="G22" s="27"/>
       <c r="H22" s="32"/>
@@ -1180,12 +1186,10 @@
     </row>
     <row r="23" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="53"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="19"/>
-      <c r="E23" s="45" t="s">
-        <v>20</v>
-      </c>
+      <c r="E23" s="45"/>
       <c r="F23" s="48"/>
       <c r="G23" s="27"/>
       <c r="H23" s="32"/>
@@ -1193,8 +1197,8 @@
     </row>
     <row r="24" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="53"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="19"/>
       <c r="E24" s="45"/>
       <c r="F24" s="48"/>
@@ -1204,8 +1208,8 @@
     </row>
     <row r="25" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="53"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="19"/>
       <c r="E25" s="45"/>
       <c r="F25" s="46"/>
@@ -1216,9 +1220,9 @@
     <row r="26" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="53"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="54"/>
+      <c r="E26" s="53"/>
       <c r="F26" s="4"/>
       <c r="G26" s="19"/>
       <c r="H26" s="32"/>
@@ -1226,51 +1230,51 @@
     </row>
     <row r="27" spans="1:9" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
-      <c r="B27" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="56">
+      <c r="B27" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="55">
         <f>SUM(C10:C13)</f>
-        <v>150000</v>
+        <v>371250</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="E27" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="58">
+      <c r="E27" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="57">
         <f>SUM(F10:F25)</f>
-        <v>172375</v>
+        <v>222875</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="32"/>
       <c r="I27" s="33"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="59"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="61"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="60"/>
       <c r="H28" s="32"/>
       <c r="I28" s="33"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="62"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
       <c r="H29" s="33"/>
       <c r="I29" s="33"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="64"/>
+      <c r="C30" s="63"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
@@ -1281,7 +1285,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="64"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="33"/>
@@ -1290,7 +1294,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="64"/>
+      <c r="C32" s="63"/>
       <c r="D32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="33"/>
@@ -1299,7 +1303,7 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
-      <c r="C33" s="64"/>
+      <c r="C33" s="63"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1310,7 +1314,7 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
-      <c r="C34" s="64"/>
+      <c r="C34" s="63"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1321,7 +1325,7 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
-      <c r="C35" s="64"/>
+      <c r="C35" s="63"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1332,7 +1336,7 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="64"/>
+      <c r="C36" s="63"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
@@ -1343,7 +1347,7 @@
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
-      <c r="C37" s="64"/>
+      <c r="C37" s="63"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1354,7 +1358,7 @@
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
-      <c r="C38" s="64"/>
+      <c r="C38" s="63"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1365,7 +1369,7 @@
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
-      <c r="C39" s="64"/>
+      <c r="C39" s="63"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
@@ -1376,7 +1380,7 @@
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
-      <c r="C40" s="64"/>
+      <c r="C40" s="63"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
@@ -1387,7 +1391,7 @@
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
-      <c r="C41" s="64"/>
+      <c r="C41" s="63"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
@@ -1398,7 +1402,7 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
-      <c r="C42" s="64"/>
+      <c r="C42" s="63"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
@@ -1409,7 +1413,7 @@
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
-      <c r="C43" s="64"/>
+      <c r="C43" s="63"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -1420,7 +1424,7 @@
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
-      <c r="C44" s="64"/>
+      <c r="C44" s="63"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -1431,7 +1435,7 @@
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
-      <c r="C45" s="64"/>
+      <c r="C45" s="63"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
@@ -1442,7 +1446,7 @@
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
-      <c r="C46" s="64"/>
+      <c r="C46" s="63"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
@@ -1453,7 +1457,7 @@
     <row r="47" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
-      <c r="C47" s="64"/>
+      <c r="C47" s="63"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
@@ -1464,7 +1468,7 @@
     <row r="48" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
-      <c r="C48" s="64"/>
+      <c r="C48" s="63"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
@@ -1475,7 +1479,7 @@
     <row r="49" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="64"/>
+      <c r="C49" s="63"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
@@ -1486,7 +1490,7 @@
     <row r="50" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
-      <c r="C50" s="64"/>
+      <c r="C50" s="63"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
@@ -1497,7 +1501,7 @@
     <row r="51" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
-      <c r="C51" s="64"/>
+      <c r="C51" s="63"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
@@ -1508,7 +1512,7 @@
     <row r="52" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
-      <c r="C52" s="64"/>
+      <c r="C52" s="63"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
@@ -1519,7 +1523,7 @@
     <row r="53" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
-      <c r="C53" s="64"/>
+      <c r="C53" s="63"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
@@ -1530,7 +1534,7 @@
     <row r="54" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
-      <c r="C54" s="64"/>
+      <c r="C54" s="63"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
@@ -1541,7 +1545,7 @@
     <row r="55" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
-      <c r="C55" s="64"/>
+      <c r="C55" s="63"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
@@ -1552,7 +1556,7 @@
     <row r="56" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
-      <c r="C56" s="64"/>
+      <c r="C56" s="63"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
@@ -1563,7 +1567,7 @@
     <row r="57" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
-      <c r="C57" s="64"/>
+      <c r="C57" s="63"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
@@ -1574,7 +1578,7 @@
     <row r="58" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
-      <c r="C58" s="64"/>
+      <c r="C58" s="63"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
@@ -1585,7 +1589,7 @@
     <row r="59" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8"/>
       <c r="B59" s="33"/>
-      <c r="C59" s="65"/>
+      <c r="C59" s="64"/>
       <c r="D59" s="8"/>
       <c r="E59" s="33"/>
       <c r="F59" s="33"/>
@@ -1596,7 +1600,7 @@
     <row r="60" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="B60" s="33"/>
-      <c r="C60" s="65"/>
+      <c r="C60" s="64"/>
       <c r="D60" s="8"/>
       <c r="E60" s="33"/>
       <c r="F60" s="33"/>
@@ -1607,7 +1611,7 @@
     <row r="61" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="8"/>
       <c r="B61" s="33"/>
-      <c r="C61" s="65"/>
+      <c r="C61" s="64"/>
       <c r="D61" s="33"/>
       <c r="E61" s="33"/>
       <c r="F61" s="33"/>
@@ -1618,7 +1622,7 @@
     <row r="62" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="B62" s="33"/>
-      <c r="C62" s="65"/>
+      <c r="C62" s="64"/>
       <c r="D62" s="33"/>
       <c r="E62" s="33"/>
       <c r="F62" s="33"/>
@@ -1629,7 +1633,7 @@
     <row r="63" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
-      <c r="C63" s="64"/>
+      <c r="C63" s="63"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
@@ -1640,7 +1644,7 @@
     <row r="64" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
-      <c r="C64" s="64"/>
+      <c r="C64" s="63"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
@@ -1651,7 +1655,7 @@
     <row r="65" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
-      <c r="C65" s="64"/>
+      <c r="C65" s="63"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
@@ -1662,7 +1666,7 @@
     <row r="66" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
-      <c r="C66" s="64"/>
+      <c r="C66" s="63"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
@@ -1673,7 +1677,7 @@
     <row r="67" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
-      <c r="C67" s="64"/>
+      <c r="C67" s="63"/>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
@@ -1684,7 +1688,7 @@
     <row r="68" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
-      <c r="C68" s="64"/>
+      <c r="C68" s="63"/>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
@@ -1695,7 +1699,7 @@
     <row r="69" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
-      <c r="C69" s="64"/>
+      <c r="C69" s="63"/>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
@@ -1706,7 +1710,7 @@
     <row r="70" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
-      <c r="C70" s="64"/>
+      <c r="C70" s="63"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
@@ -1717,7 +1721,7 @@
     <row r="71" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
-      <c r="C71" s="64"/>
+      <c r="C71" s="63"/>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
@@ -1728,7 +1732,7 @@
     <row r="72" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
-      <c r="C72" s="64"/>
+      <c r="C72" s="63"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
@@ -1739,7 +1743,7 @@
     <row r="73" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
-      <c r="C73" s="64"/>
+      <c r="C73" s="63"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
@@ -1750,7 +1754,7 @@
     <row r="74" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
-      <c r="C74" s="64"/>
+      <c r="C74" s="63"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
@@ -1761,7 +1765,7 @@
     <row r="75" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
-      <c r="C75" s="64"/>
+      <c r="C75" s="63"/>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
@@ -1772,7 +1776,7 @@
     <row r="76" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
-      <c r="C76" s="64"/>
+      <c r="C76" s="63"/>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
@@ -1790,108 +1794,150 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="68"/>
+    <col min="3" max="3" width="9.140625" style="67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="68"/>
-    </row>
-    <row r="2" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="68"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="67"/>
+    </row>
+    <row r="2" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="67"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <f>B9*5</f>
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>150000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6">
-        <v>2000</v>
-      </c>
-      <c r="C6" s="68" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="68">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="67"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <f>C9*D9</f>
+        <v>310</v>
+      </c>
+      <c r="C9" s="67">
+        <v>1.24</v>
+      </c>
+      <c r="D9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>33</v>
       </c>
-      <c r="B9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B11">
+        <f>30000</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B10">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
       <c r="B12">
-        <v>700</v>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update budget after remarks Laura
</commit_message>
<xml_diff>
--- a/Budget/owasp-devseccon-summit-budget.xlsx
+++ b/Budget/owasp-devseccon-summit-budget.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="readme1st" sheetId="3" r:id="rId1"/>
     <sheet name="summit 2017 budget" sheetId="1" r:id="rId2"/>
     <sheet name="Assumptions" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Estimated profit</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Internet uplink</t>
+  </si>
+  <si>
+    <t>ticket per paying attendee (excl travel)</t>
   </si>
 </sst>
 </file>
@@ -540,17 +543,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -897,10 +900,10 @@
     </row>
     <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="70"/>
+      <c r="C2" s="72"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="66">
@@ -951,7 +954,7 @@
       </c>
       <c r="F5" s="30">
         <f>C27-F27</f>
-        <v>35125</v>
+        <v>37000</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="7"/>
@@ -1020,7 +1023,7 @@
       <c r="E10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="70">
         <f>(Assumptions!B6+Assumptions!B7)*Assumptions!B8*Assumptions!B9</f>
         <v>178250</v>
       </c>
@@ -1041,7 +1044,7 @@
       <c r="E11" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="72" t="s">
+      <c r="F11" s="70" t="s">
         <v>35</v>
       </c>
       <c r="G11" s="47"/>
@@ -1061,7 +1064,7 @@
       <c r="E12" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="72">
+      <c r="F12" s="70">
         <f>Assumptions!B7*Assumptions!B10</f>
         <v>45000</v>
       </c>
@@ -1079,10 +1082,10 @@
         <v>75000</v>
       </c>
       <c r="D13" s="27"/>
-      <c r="E13" s="71" t="s">
+      <c r="E13" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="72">
+      <c r="F13" s="70">
         <f>Assumptions!B17</f>
         <v>30000</v>
       </c>
@@ -1098,7 +1101,7 @@
       <c r="E14" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="72">
+      <c r="F14" s="70">
         <v>1000</v>
       </c>
       <c r="G14" s="47"/>
@@ -1111,7 +1114,7 @@
       <c r="E15" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="72">
+      <c r="F15" s="70">
         <v>1000</v>
       </c>
       <c r="G15" s="47"/>
@@ -1126,7 +1129,7 @@
       <c r="E16" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="72">
+      <c r="F16" s="70">
         <f>(Assumptions!B3+Assumptions!B6+Assumptions!B7)*Assumptions!B13</f>
         <v>6250</v>
       </c>
@@ -1142,9 +1145,9 @@
       <c r="E17" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="72">
+      <c r="F17" s="70">
         <f>(Assumptions!B3+Assumptions!B7+Assumptions!B6)*Assumptions!B14</f>
-        <v>3750</v>
+        <v>1875</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="32"/>
@@ -1158,7 +1161,7 @@
       <c r="E18" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="72">
+      <c r="F18" s="70">
         <f>Assumptions!B15</f>
         <v>3000</v>
       </c>
@@ -1174,7 +1177,7 @@
       <c r="E19" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="72">
+      <c r="F19" s="70">
         <f>C4*Assumptions!B16</f>
         <v>625</v>
       </c>
@@ -1190,7 +1193,7 @@
       <c r="E20" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="72">
+      <c r="F20" s="70">
         <f>Assumptions!B20</f>
         <v>3000</v>
       </c>
@@ -1206,7 +1209,7 @@
       <c r="E21" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="72">
+      <c r="F21" s="70">
         <f>Assumptions!B21</f>
         <v>10000</v>
       </c>
@@ -1284,7 +1287,7 @@
       </c>
       <c r="F27" s="57">
         <f>SUM(F10:F25)</f>
-        <v>281875</v>
+        <v>280000</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="32"/>
@@ -1835,10 +1838,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1953,7 +1956,7 @@
         <v>38</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2016,6 +2019,15 @@
       </c>
       <c r="C21" s="67" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22">
+        <f>B9*B8</f>
+        <v>1550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>